<commit_message>
- fixed error when dynamic data cannot be resolved during the initialization of an execution. This fix stabilize the   execution.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_base_part1.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_base_part1.data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11206"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10502"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-core/src/test/resources/showcase/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C521B7-961E-0D45-972B-700C25D244F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView tabRatio="500" windowHeight="10280" windowWidth="33600" xWindow="8380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-20560"/>
+    <workbookView xWindow="8380" yWindow="440" windowWidth="33600" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="#default" r:id="rId1" sheetId="2"/>
-    <sheet name="sentry_function_projectfile" r:id="rId2" sheetId="3"/>
+    <sheet name="#default" sheetId="2" r:id="rId1"/>
+    <sheet name="sentry_function_projectfile" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -41,7 +42,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -54,15 +55,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>sentry.pollWaitMs</t>
-  </si>
-  <si>
-    <t>sentry.textDelim</t>
   </si>
   <si>
     <t>,</t>
@@ -74,31 +69,7 @@
     <t>var2</t>
   </si>
   <si>
-    <t>sentry.scope.mailTo</t>
-  </si>
-  <si>
-    <t>sentry.scope.executionMode</t>
-  </si>
-  <si>
-    <t>local</t>
-  </si>
-  <si>
-    <t>sentry.scope.iteration</t>
-  </si>
-  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>sentry.scope.fallbackToPrevious</t>
-  </si>
-  <si>
-    <t>sentry.delayBetweenStepsMs</t>
-  </si>
-  <si>
-    <t>sentry.failFast</t>
-  </si>
-  <si>
-    <t>sentry.verbose</t>
   </si>
   <si>
     <t>false</t>
@@ -167,13 +138,7 @@
     <t>14</t>
   </si>
   <si>
-    <t>sentry.elapsedTimeSLA</t>
-  </si>
-  <si>
     <t>6000</t>
-  </si>
-  <si>
-    <t>sentry.scriptRef.startDate</t>
   </si>
   <si>
     <t>${startYear}-${startMonth}-${startDate}</t>
@@ -195,9 +160,6 @@
   </si>
   <si>
     <t>Hello World</t>
-  </si>
-  <si>
-    <t>nexial.scope.executionMode</t>
   </si>
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
@@ -234,8 +196,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="20">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -288,84 +249,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="3E511F"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="5A5A32"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="12284A"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="0000FF"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="006100"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="808080"/>
-      <u val="none"/>
-    </font>
   </fonts>
-  <fills count="24">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,127 +263,8 @@
         <bgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -521,299 +287,69 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin">
-        <color rgb="C8B4B4"/>
-      </right>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin">
-        <color rgb="DCDCDC"/>
-      </right>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDCDCD"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="C3C3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="5" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="17" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="21" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="21" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="4"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="6"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="8"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="10"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="12"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="3"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="5"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="7"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="9"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="11"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -1106,7 +642,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1125,7 +661,7 @@
       <sheetName val="#system"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData refreshError="1" sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1136,10 +672,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1174,7 +710,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -1209,7 +745,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1303,21 +839,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1334,7 +870,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1386,35 +922,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAB21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AAA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -1622,7 +1158,7 @@
       <c r="GX1"/>
       <c r="GY1"/>
       <c r="GZ1"/>
-      <c r="HA1"/>
+      <c r="HA1" s="7"/>
       <c r="HB1"/>
       <c r="HC1"/>
       <c r="HD1"/>
@@ -2116,13 +1652,14 @@
       <c r="ZX1"/>
       <c r="ZY1"/>
       <c r="ZZ1"/>
+      <c r="AAA1" s="7"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2827,12 +2364,10 @@
       <c r="AAA2" s="7"/>
     </row>
     <row r="3" spans="1:703">
-      <c r="A3" s="1" t="s">
-        <v>49</v>
+      <c r="A3" s="6" t="s">
+        <v>37</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
@@ -3536,10 +3071,12 @@
       <c r="AAA3" s="7"/>
     </row>
     <row r="4" spans="1:703">
-      <c r="A4" s="6" t="s">
-        <v>50</v>
+      <c r="A4" s="1" t="s">
+        <v>38</v>
       </c>
-      <c r="B4"/>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
@@ -3746,7 +3283,7 @@
       <c r="GX4"/>
       <c r="GY4"/>
       <c r="GZ4"/>
-      <c r="HA4" s="7"/>
+      <c r="HA4" s="4"/>
       <c r="HB4"/>
       <c r="HC4"/>
       <c r="HD4"/>
@@ -4240,14 +3777,14 @@
       <c r="ZX4"/>
       <c r="ZY4"/>
       <c r="ZZ4"/>
-      <c r="AAA4" s="7"/>
+      <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -4953,10 +4490,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -5662,10 +5199,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -6371,10 +5908,10 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -7080,10 +6617,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -7789,10 +7326,10 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -8498,13 +8035,15 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
+      <c r="B11" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="C11"/>
-      <c r="D11"/>
+      <c r="D11" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
@@ -8709,7 +8248,7 @@
       <c r="GX11"/>
       <c r="GY11"/>
       <c r="GZ11"/>
-      <c r="HA11" s="4"/>
+      <c r="HA11"/>
       <c r="HB11"/>
       <c r="HC11"/>
       <c r="HD11"/>
@@ -9203,18 +8742,19 @@
       <c r="ZX11"/>
       <c r="ZY11"/>
       <c r="ZZ11"/>
-      <c r="AAA11" s="5"/>
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12"/>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D12" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -9917,16 +9457,16 @@
     </row>
     <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -10629,16 +10169,16 @@
     </row>
     <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>22</v>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -11341,17 +10881,15 @@
     </row>
     <row r="15" spans="1:703">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
@@ -12053,13 +11591,13 @@
     </row>
     <row r="16" spans="1:703">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
@@ -12761,15 +12299,15 @@
       <c r="ZY16"/>
       <c r="ZZ16"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:702">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -13471,16 +13009,14 @@
       <c r="ZY17"/>
       <c r="ZZ17"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:702">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -14181,12 +13717,12 @@
       <c r="ZY18"/>
       <c r="ZZ18"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:702">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -14889,12 +14425,12 @@
       <c r="ZY19"/>
       <c r="ZZ19"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:702">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -15597,807 +15133,99 @@
       <c r="ZY20"/>
       <c r="ZZ20"/>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21"/>
-      <c r="S21"/>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
-      <c r="W21"/>
-      <c r="X21"/>
-      <c r="Y21"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
-      <c r="AB21"/>
-      <c r="AC21"/>
-      <c r="AD21"/>
-      <c r="AE21"/>
-      <c r="AF21"/>
-      <c r="AG21"/>
-      <c r="AH21"/>
-      <c r="AI21"/>
-      <c r="AJ21"/>
-      <c r="AK21"/>
-      <c r="AL21"/>
-      <c r="AM21"/>
-      <c r="AN21"/>
-      <c r="AO21"/>
-      <c r="AP21"/>
-      <c r="AQ21"/>
-      <c r="AR21"/>
-      <c r="AS21"/>
-      <c r="AT21"/>
-      <c r="AU21"/>
-      <c r="AV21"/>
-      <c r="AW21"/>
-      <c r="AX21"/>
-      <c r="AY21"/>
-      <c r="AZ21"/>
-      <c r="BA21"/>
-      <c r="BB21"/>
-      <c r="BC21"/>
-      <c r="BD21"/>
-      <c r="BE21"/>
-      <c r="BF21"/>
-      <c r="BG21"/>
-      <c r="BH21"/>
-      <c r="BI21"/>
-      <c r="BJ21"/>
-      <c r="BK21"/>
-      <c r="BL21"/>
-      <c r="BM21"/>
-      <c r="BN21"/>
-      <c r="BO21"/>
-      <c r="BP21"/>
-      <c r="BQ21"/>
-      <c r="BR21"/>
-      <c r="BS21"/>
-      <c r="BT21"/>
-      <c r="BU21"/>
-      <c r="BV21"/>
-      <c r="BW21"/>
-      <c r="BX21"/>
-      <c r="BY21"/>
-      <c r="BZ21"/>
-      <c r="CA21"/>
-      <c r="CB21"/>
-      <c r="CC21"/>
-      <c r="CD21"/>
-      <c r="CE21"/>
-      <c r="CF21"/>
-      <c r="CG21"/>
-      <c r="CH21"/>
-      <c r="CI21"/>
-      <c r="CJ21"/>
-      <c r="CK21"/>
-      <c r="CL21"/>
-      <c r="CM21"/>
-      <c r="CN21"/>
-      <c r="CO21"/>
-      <c r="CP21"/>
-      <c r="CQ21"/>
-      <c r="CR21"/>
-      <c r="CS21"/>
-      <c r="CT21"/>
-      <c r="CU21"/>
-      <c r="CV21"/>
-      <c r="CW21"/>
-      <c r="CX21"/>
-      <c r="CY21"/>
-      <c r="CZ21"/>
-      <c r="DA21"/>
-      <c r="DB21"/>
-      <c r="DC21"/>
-      <c r="DD21"/>
-      <c r="DE21"/>
-      <c r="DF21"/>
-      <c r="DG21"/>
-      <c r="DH21"/>
-      <c r="DI21"/>
-      <c r="DJ21"/>
-      <c r="DK21"/>
-      <c r="DL21"/>
-      <c r="DM21"/>
-      <c r="DN21"/>
-      <c r="DO21"/>
-      <c r="DP21"/>
-      <c r="DQ21"/>
-      <c r="DR21"/>
-      <c r="DS21"/>
-      <c r="DT21"/>
-      <c r="DU21"/>
-      <c r="DV21"/>
-      <c r="DW21"/>
-      <c r="DX21"/>
-      <c r="DY21"/>
-      <c r="DZ21"/>
-      <c r="EA21"/>
-      <c r="EB21"/>
-      <c r="EC21"/>
-      <c r="ED21"/>
-      <c r="EE21"/>
-      <c r="EF21"/>
-      <c r="EG21"/>
-      <c r="EH21"/>
-      <c r="EI21"/>
-      <c r="EJ21"/>
-      <c r="EK21"/>
-      <c r="EL21"/>
-      <c r="EM21"/>
-      <c r="EN21"/>
-      <c r="EO21"/>
-      <c r="EP21"/>
-      <c r="EQ21"/>
-      <c r="ER21"/>
-      <c r="ES21"/>
-      <c r="ET21"/>
-      <c r="EU21"/>
-      <c r="EV21"/>
-      <c r="EW21"/>
-      <c r="EX21"/>
-      <c r="EY21"/>
-      <c r="EZ21"/>
-      <c r="FA21"/>
-      <c r="FB21"/>
-      <c r="FC21"/>
-      <c r="FD21"/>
-      <c r="FE21"/>
-      <c r="FF21"/>
-      <c r="FG21"/>
-      <c r="FH21"/>
-      <c r="FI21"/>
-      <c r="FJ21"/>
-      <c r="FK21"/>
-      <c r="FL21"/>
-      <c r="FM21"/>
-      <c r="FN21"/>
-      <c r="FO21"/>
-      <c r="FP21"/>
-      <c r="FQ21"/>
-      <c r="FR21"/>
-      <c r="FS21"/>
-      <c r="FT21"/>
-      <c r="FU21"/>
-      <c r="FV21"/>
-      <c r="FW21"/>
-      <c r="FX21"/>
-      <c r="FY21"/>
-      <c r="FZ21"/>
-      <c r="GA21"/>
-      <c r="GB21"/>
-      <c r="GC21"/>
-      <c r="GD21"/>
-      <c r="GE21"/>
-      <c r="GF21"/>
-      <c r="GG21"/>
-      <c r="GH21"/>
-      <c r="GI21"/>
-      <c r="GJ21"/>
-      <c r="GK21"/>
-      <c r="GL21"/>
-      <c r="GM21"/>
-      <c r="GN21"/>
-      <c r="GO21"/>
-      <c r="GP21"/>
-      <c r="GQ21"/>
-      <c r="GR21"/>
-      <c r="GS21"/>
-      <c r="GT21"/>
-      <c r="GU21"/>
-      <c r="GV21"/>
-      <c r="GW21"/>
-      <c r="GX21"/>
-      <c r="GY21"/>
-      <c r="GZ21"/>
-      <c r="HA21"/>
-      <c r="HB21"/>
-      <c r="HC21"/>
-      <c r="HD21"/>
-      <c r="HE21"/>
-      <c r="HF21"/>
-      <c r="HG21"/>
-      <c r="HH21"/>
-      <c r="HI21"/>
-      <c r="HJ21"/>
-      <c r="HK21"/>
-      <c r="HL21"/>
-      <c r="HM21"/>
-      <c r="HN21"/>
-      <c r="HO21"/>
-      <c r="HP21"/>
-      <c r="HQ21"/>
-      <c r="HR21"/>
-      <c r="HS21"/>
-      <c r="HT21"/>
-      <c r="HU21"/>
-      <c r="HV21"/>
-      <c r="HW21"/>
-      <c r="HX21"/>
-      <c r="HY21"/>
-      <c r="HZ21"/>
-      <c r="IA21"/>
-      <c r="IB21"/>
-      <c r="IC21"/>
-      <c r="ID21"/>
-      <c r="IE21"/>
-      <c r="IF21"/>
-      <c r="IG21"/>
-      <c r="IH21"/>
-      <c r="II21"/>
-      <c r="IJ21"/>
-      <c r="IK21"/>
-      <c r="IL21"/>
-      <c r="IM21"/>
-      <c r="IN21"/>
-      <c r="IO21"/>
-      <c r="IP21"/>
-      <c r="IQ21"/>
-      <c r="IR21"/>
-      <c r="IS21"/>
-      <c r="IT21"/>
-      <c r="IU21"/>
-      <c r="IV21"/>
-      <c r="IW21"/>
-      <c r="IX21"/>
-      <c r="IY21"/>
-      <c r="IZ21"/>
-      <c r="JA21"/>
-      <c r="JB21"/>
-      <c r="JC21"/>
-      <c r="JD21"/>
-      <c r="JE21"/>
-      <c r="JF21"/>
-      <c r="JG21"/>
-      <c r="JH21"/>
-      <c r="JI21"/>
-      <c r="JJ21"/>
-      <c r="JK21"/>
-      <c r="JL21"/>
-      <c r="JM21"/>
-      <c r="JN21"/>
-      <c r="JO21"/>
-      <c r="JP21"/>
-      <c r="JQ21"/>
-      <c r="JR21"/>
-      <c r="JS21"/>
-      <c r="JT21"/>
-      <c r="JU21"/>
-      <c r="JV21"/>
-      <c r="JW21"/>
-      <c r="JX21"/>
-      <c r="JY21"/>
-      <c r="JZ21"/>
-      <c r="KA21"/>
-      <c r="KB21"/>
-      <c r="KC21"/>
-      <c r="KD21"/>
-      <c r="KE21"/>
-      <c r="KF21"/>
-      <c r="KG21"/>
-      <c r="KH21"/>
-      <c r="KI21"/>
-      <c r="KJ21"/>
-      <c r="KK21"/>
-      <c r="KL21"/>
-      <c r="KM21"/>
-      <c r="KN21"/>
-      <c r="KO21"/>
-      <c r="KP21"/>
-      <c r="KQ21"/>
-      <c r="KR21"/>
-      <c r="KS21"/>
-      <c r="KT21"/>
-      <c r="KU21"/>
-      <c r="KV21"/>
-      <c r="KW21"/>
-      <c r="KX21"/>
-      <c r="KY21"/>
-      <c r="KZ21"/>
-      <c r="LA21"/>
-      <c r="LB21"/>
-      <c r="LC21"/>
-      <c r="LD21"/>
-      <c r="LE21"/>
-      <c r="LF21"/>
-      <c r="LG21"/>
-      <c r="LH21"/>
-      <c r="LI21"/>
-      <c r="LJ21"/>
-      <c r="LK21"/>
-      <c r="LL21"/>
-      <c r="LM21"/>
-      <c r="LN21"/>
-      <c r="LO21"/>
-      <c r="LP21"/>
-      <c r="LQ21"/>
-      <c r="LR21"/>
-      <c r="LS21"/>
-      <c r="LT21"/>
-      <c r="LU21"/>
-      <c r="LV21"/>
-      <c r="LW21"/>
-      <c r="LX21"/>
-      <c r="LY21"/>
-      <c r="LZ21"/>
-      <c r="MA21"/>
-      <c r="MB21"/>
-      <c r="MC21"/>
-      <c r="MD21"/>
-      <c r="ME21"/>
-      <c r="MF21"/>
-      <c r="MG21"/>
-      <c r="MH21"/>
-      <c r="MI21"/>
-      <c r="MJ21"/>
-      <c r="MK21"/>
-      <c r="ML21"/>
-      <c r="MM21"/>
-      <c r="MN21"/>
-      <c r="MO21"/>
-      <c r="MP21"/>
-      <c r="MQ21"/>
-      <c r="MR21"/>
-      <c r="MS21"/>
-      <c r="MT21"/>
-      <c r="MU21"/>
-      <c r="MV21"/>
-      <c r="MW21"/>
-      <c r="MX21"/>
-      <c r="MY21"/>
-      <c r="MZ21"/>
-      <c r="NA21"/>
-      <c r="NB21"/>
-      <c r="NC21"/>
-      <c r="ND21"/>
-      <c r="NE21"/>
-      <c r="NF21"/>
-      <c r="NG21"/>
-      <c r="NH21"/>
-      <c r="NI21"/>
-      <c r="NJ21"/>
-      <c r="NK21"/>
-      <c r="NL21"/>
-      <c r="NM21"/>
-      <c r="NN21"/>
-      <c r="NO21"/>
-      <c r="NP21"/>
-      <c r="NQ21"/>
-      <c r="NR21"/>
-      <c r="NS21"/>
-      <c r="NT21"/>
-      <c r="NU21"/>
-      <c r="NV21"/>
-      <c r="NW21"/>
-      <c r="NX21"/>
-      <c r="NY21"/>
-      <c r="NZ21"/>
-      <c r="OA21"/>
-      <c r="OB21"/>
-      <c r="OC21"/>
-      <c r="OD21"/>
-      <c r="OE21"/>
-      <c r="OF21"/>
-      <c r="OG21"/>
-      <c r="OH21"/>
-      <c r="OI21"/>
-      <c r="OJ21"/>
-      <c r="OK21"/>
-      <c r="OL21"/>
-      <c r="OM21"/>
-      <c r="ON21"/>
-      <c r="OO21"/>
-      <c r="OP21"/>
-      <c r="OQ21"/>
-      <c r="OR21"/>
-      <c r="OS21"/>
-      <c r="OT21"/>
-      <c r="OU21"/>
-      <c r="OV21"/>
-      <c r="OW21"/>
-      <c r="OX21"/>
-      <c r="OY21"/>
-      <c r="OZ21"/>
-      <c r="PA21"/>
-      <c r="PB21"/>
-      <c r="PC21"/>
-      <c r="PD21"/>
-      <c r="PE21"/>
-      <c r="PF21"/>
-      <c r="PG21"/>
-      <c r="PH21"/>
-      <c r="PI21"/>
-      <c r="PJ21"/>
-      <c r="PK21"/>
-      <c r="PL21"/>
-      <c r="PM21"/>
-      <c r="PN21"/>
-      <c r="PO21"/>
-      <c r="PP21"/>
-      <c r="PQ21"/>
-      <c r="PR21"/>
-      <c r="PS21"/>
-      <c r="PT21"/>
-      <c r="PU21"/>
-      <c r="PV21"/>
-      <c r="PW21"/>
-      <c r="PX21"/>
-      <c r="PY21"/>
-      <c r="PZ21"/>
-      <c r="QA21"/>
-      <c r="QB21"/>
-      <c r="QC21"/>
-      <c r="QD21"/>
-      <c r="QE21"/>
-      <c r="QF21"/>
-      <c r="QG21"/>
-      <c r="QH21"/>
-      <c r="QI21"/>
-      <c r="QJ21"/>
-      <c r="QK21"/>
-      <c r="QL21"/>
-      <c r="QM21"/>
-      <c r="QN21"/>
-      <c r="QO21"/>
-      <c r="QP21"/>
-      <c r="QQ21"/>
-      <c r="QR21"/>
-      <c r="QS21"/>
-      <c r="QT21"/>
-      <c r="QU21"/>
-      <c r="QV21"/>
-      <c r="QW21"/>
-      <c r="QX21"/>
-      <c r="QY21"/>
-      <c r="QZ21"/>
-      <c r="RA21"/>
-      <c r="RB21"/>
-      <c r="RC21"/>
-      <c r="RD21"/>
-      <c r="RE21"/>
-      <c r="RF21"/>
-      <c r="RG21"/>
-      <c r="RH21"/>
-      <c r="RI21"/>
-      <c r="RJ21"/>
-      <c r="RK21"/>
-      <c r="RL21"/>
-      <c r="RM21"/>
-      <c r="RN21"/>
-      <c r="RO21"/>
-      <c r="RP21"/>
-      <c r="RQ21"/>
-      <c r="RR21"/>
-      <c r="RS21"/>
-      <c r="RT21"/>
-      <c r="RU21"/>
-      <c r="RV21"/>
-      <c r="RW21"/>
-      <c r="RX21"/>
-      <c r="RY21"/>
-      <c r="RZ21"/>
-      <c r="SA21"/>
-      <c r="SB21"/>
-      <c r="SC21"/>
-      <c r="SD21"/>
-      <c r="SE21"/>
-      <c r="SF21"/>
-      <c r="SG21"/>
-      <c r="SH21"/>
-      <c r="SI21"/>
-      <c r="SJ21"/>
-      <c r="SK21"/>
-      <c r="SL21"/>
-      <c r="SM21"/>
-      <c r="SN21"/>
-      <c r="SO21"/>
-      <c r="SP21"/>
-      <c r="SQ21"/>
-      <c r="SR21"/>
-      <c r="SS21"/>
-      <c r="ST21"/>
-      <c r="SU21"/>
-      <c r="SV21"/>
-      <c r="SW21"/>
-      <c r="SX21"/>
-      <c r="SY21"/>
-      <c r="SZ21"/>
-      <c r="TA21"/>
-      <c r="TB21"/>
-      <c r="TC21"/>
-      <c r="TD21"/>
-      <c r="TE21"/>
-      <c r="TF21"/>
-      <c r="TG21"/>
-      <c r="TH21"/>
-      <c r="TI21"/>
-      <c r="TJ21"/>
-      <c r="TK21"/>
-      <c r="TL21"/>
-      <c r="TM21"/>
-      <c r="TN21"/>
-      <c r="TO21"/>
-      <c r="TP21"/>
-      <c r="TQ21"/>
-      <c r="TR21"/>
-      <c r="TS21"/>
-      <c r="TT21"/>
-      <c r="TU21"/>
-      <c r="TV21"/>
-      <c r="TW21"/>
-      <c r="TX21"/>
-      <c r="TY21"/>
-      <c r="TZ21"/>
-      <c r="UA21"/>
-      <c r="UB21"/>
-      <c r="UC21"/>
-      <c r="UD21"/>
-      <c r="UE21"/>
-      <c r="UF21"/>
-      <c r="UG21"/>
-      <c r="UH21"/>
-      <c r="UI21"/>
-      <c r="UJ21"/>
-      <c r="UK21"/>
-      <c r="UL21"/>
-      <c r="UM21"/>
-      <c r="UN21"/>
-      <c r="UO21"/>
-      <c r="UP21"/>
-      <c r="UQ21"/>
-      <c r="UR21"/>
-      <c r="US21"/>
-      <c r="UT21"/>
-      <c r="UU21"/>
-      <c r="UV21"/>
-      <c r="UW21"/>
-      <c r="UX21"/>
-      <c r="UY21"/>
-      <c r="UZ21"/>
-      <c r="VA21"/>
-      <c r="VB21"/>
-      <c r="VC21"/>
-      <c r="VD21"/>
-      <c r="VE21"/>
-      <c r="VF21"/>
-      <c r="VG21"/>
-      <c r="VH21"/>
-      <c r="VI21"/>
-      <c r="VJ21"/>
-      <c r="VK21"/>
-      <c r="VL21"/>
-      <c r="VM21"/>
-      <c r="VN21"/>
-      <c r="VO21"/>
-      <c r="VP21"/>
-      <c r="VQ21"/>
-      <c r="VR21"/>
-      <c r="VS21"/>
-      <c r="VT21"/>
-      <c r="VU21"/>
-      <c r="VV21"/>
-      <c r="VW21"/>
-      <c r="VX21"/>
-      <c r="VY21"/>
-      <c r="VZ21"/>
-      <c r="WA21"/>
-      <c r="WB21"/>
-      <c r="WC21"/>
-      <c r="WD21"/>
-      <c r="WE21"/>
-      <c r="WF21"/>
-      <c r="WG21"/>
-      <c r="WH21"/>
-      <c r="WI21"/>
-      <c r="WJ21"/>
-      <c r="WK21"/>
-      <c r="WL21"/>
-      <c r="WM21"/>
-      <c r="WN21"/>
-      <c r="WO21"/>
-      <c r="WP21"/>
-      <c r="WQ21"/>
-      <c r="WR21"/>
-      <c r="WS21"/>
-      <c r="WT21"/>
-      <c r="WU21"/>
-      <c r="WV21"/>
-      <c r="WW21"/>
-      <c r="WX21"/>
-      <c r="WY21"/>
-      <c r="WZ21"/>
-      <c r="XA21"/>
-      <c r="XB21"/>
-      <c r="XC21"/>
-      <c r="XD21"/>
-      <c r="XE21"/>
-      <c r="XF21"/>
-      <c r="XG21"/>
-      <c r="XH21"/>
-      <c r="XI21"/>
-      <c r="XJ21"/>
-      <c r="XK21"/>
-      <c r="XL21"/>
-      <c r="XM21"/>
-      <c r="XN21"/>
-      <c r="XO21"/>
-      <c r="XP21"/>
-      <c r="XQ21"/>
-      <c r="XR21"/>
-      <c r="XS21"/>
-      <c r="XT21"/>
-      <c r="XU21"/>
-      <c r="XV21"/>
-      <c r="XW21"/>
-      <c r="XX21"/>
-      <c r="XY21"/>
-      <c r="XZ21"/>
-      <c r="YA21"/>
-      <c r="YB21"/>
-      <c r="YC21"/>
-      <c r="YD21"/>
-      <c r="YE21"/>
-      <c r="YF21"/>
-      <c r="YG21"/>
-      <c r="YH21"/>
-      <c r="YI21"/>
-      <c r="YJ21"/>
-      <c r="YK21"/>
-      <c r="YL21"/>
-      <c r="YM21"/>
-      <c r="YN21"/>
-      <c r="YO21"/>
-      <c r="YP21"/>
-      <c r="YQ21"/>
-      <c r="YR21"/>
-      <c r="YS21"/>
-      <c r="YT21"/>
-      <c r="YU21"/>
-      <c r="YV21"/>
-      <c r="YW21"/>
-      <c r="YX21"/>
-      <c r="YY21"/>
-      <c r="YZ21"/>
-      <c r="ZA21"/>
-      <c r="ZB21"/>
-      <c r="ZC21"/>
-      <c r="ZD21"/>
-      <c r="ZE21"/>
-      <c r="ZF21"/>
-      <c r="ZG21"/>
-      <c r="ZH21"/>
-      <c r="ZI21"/>
-      <c r="ZJ21"/>
-      <c r="ZK21"/>
-      <c r="ZL21"/>
-      <c r="ZM21"/>
-      <c r="ZN21"/>
-      <c r="ZO21"/>
-      <c r="ZP21"/>
-      <c r="ZQ21"/>
-      <c r="ZR21"/>
-      <c r="ZS21"/>
-      <c r="ZT21"/>
-      <c r="ZU21"/>
-      <c r="ZV21"/>
-      <c r="ZW21"/>
-      <c r="ZX21"/>
-      <c r="ZY21"/>
-      <c r="ZZ21"/>
-    </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
-  <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule dxfId="20" operator="beginsWith" priority="20" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A22:A1048576 A1:A18">
+    <cfRule type="beginsWith" dxfId="20" priority="20" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="19" operator="beginsWith" priority="21" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="19" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="18" priority="22" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="22" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B11 B15:B1048576">
-    <cfRule dxfId="17" priority="23" stopIfTrue="1" type="expression">
+  <conditionalFormatting sqref="B14:B1048576 B1:B10">
+    <cfRule type="expression" dxfId="17" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="16" priority="24" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="24">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:B14">
-    <cfRule dxfId="15" priority="18" stopIfTrue="1" type="expression">
+  <conditionalFormatting sqref="B11:B13">
+    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="14" priority="19" type="notContainsBlanks">
-      <formula>LEN(TRIM(B12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule dxfId="13" priority="13" stopIfTrue="1" type="expression">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule dxfId="12" priority="14" type="notContainsBlanks">
-      <formula>LEN(TRIM(B14))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="14" priority="19">
+      <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="11" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="10" priority="12" type="notContainsBlanks">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
-    <cfRule dxfId="9" priority="9" stopIfTrue="1" type="expression">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule dxfId="8" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="7" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="6" priority="8" type="notContainsBlanks">
-      <formula>LEN(TRIM(B12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
-    <cfRule dxfId="5" priority="5" stopIfTrue="1" type="expression">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule dxfId="4" priority="6" type="notContainsBlanks">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule dxfId="3" priority="3" stopIfTrue="1" type="expression">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule dxfId="2" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="1" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="0" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
+      <formula>LEN(TRIM(B11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(B12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
+      <formula>LEN(TRIM(B11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+      <formula>LEN(TRIM(B11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AAA1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -16407,713 +15235,13 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
-      <c r="R1"/>
-      <c r="S1"/>
-      <c r="T1"/>
-      <c r="U1"/>
-      <c r="V1"/>
-      <c r="W1"/>
-      <c r="X1"/>
-      <c r="Y1"/>
-      <c r="Z1"/>
-      <c r="AA1"/>
-      <c r="AB1"/>
-      <c r="AC1"/>
-      <c r="AD1"/>
-      <c r="AE1"/>
-      <c r="AF1"/>
-      <c r="AG1"/>
-      <c r="AH1"/>
-      <c r="AI1"/>
-      <c r="AJ1"/>
-      <c r="AK1"/>
-      <c r="AL1"/>
-      <c r="AM1"/>
-      <c r="AN1"/>
-      <c r="AO1"/>
-      <c r="AP1"/>
-      <c r="AQ1"/>
-      <c r="AR1"/>
-      <c r="AS1"/>
-      <c r="AT1"/>
-      <c r="AU1"/>
-      <c r="AV1"/>
-      <c r="AW1"/>
-      <c r="AX1"/>
-      <c r="AY1"/>
-      <c r="AZ1"/>
-      <c r="BA1"/>
-      <c r="BB1"/>
-      <c r="BC1"/>
-      <c r="BD1"/>
-      <c r="BE1"/>
-      <c r="BF1"/>
-      <c r="BG1"/>
-      <c r="BH1"/>
-      <c r="BI1"/>
-      <c r="BJ1"/>
-      <c r="BK1"/>
-      <c r="BL1"/>
-      <c r="BM1"/>
-      <c r="BN1"/>
-      <c r="BO1"/>
-      <c r="BP1"/>
-      <c r="BQ1"/>
-      <c r="BR1"/>
-      <c r="BS1"/>
-      <c r="BT1"/>
-      <c r="BU1"/>
-      <c r="BV1"/>
-      <c r="BW1"/>
-      <c r="BX1"/>
-      <c r="BY1"/>
-      <c r="BZ1"/>
-      <c r="CA1"/>
-      <c r="CB1"/>
-      <c r="CC1"/>
-      <c r="CD1"/>
-      <c r="CE1"/>
-      <c r="CF1"/>
-      <c r="CG1"/>
-      <c r="CH1"/>
-      <c r="CI1"/>
-      <c r="CJ1"/>
-      <c r="CK1"/>
-      <c r="CL1"/>
-      <c r="CM1"/>
-      <c r="CN1"/>
-      <c r="CO1"/>
-      <c r="CP1"/>
-      <c r="CQ1"/>
-      <c r="CR1"/>
-      <c r="CS1"/>
-      <c r="CT1"/>
-      <c r="CU1"/>
-      <c r="CV1"/>
-      <c r="CW1"/>
-      <c r="CX1"/>
-      <c r="CY1"/>
-      <c r="CZ1"/>
-      <c r="DA1"/>
-      <c r="DB1"/>
-      <c r="DC1"/>
-      <c r="DD1"/>
-      <c r="DE1"/>
-      <c r="DF1"/>
-      <c r="DG1"/>
-      <c r="DH1"/>
-      <c r="DI1"/>
-      <c r="DJ1"/>
-      <c r="DK1"/>
-      <c r="DL1"/>
-      <c r="DM1"/>
-      <c r="DN1"/>
-      <c r="DO1"/>
-      <c r="DP1"/>
-      <c r="DQ1"/>
-      <c r="DR1"/>
-      <c r="DS1"/>
-      <c r="DT1"/>
-      <c r="DU1"/>
-      <c r="DV1"/>
-      <c r="DW1"/>
-      <c r="DX1"/>
-      <c r="DY1"/>
-      <c r="DZ1"/>
-      <c r="EA1"/>
-      <c r="EB1"/>
-      <c r="EC1"/>
-      <c r="ED1"/>
-      <c r="EE1"/>
-      <c r="EF1"/>
-      <c r="EG1"/>
-      <c r="EH1"/>
-      <c r="EI1"/>
-      <c r="EJ1"/>
-      <c r="EK1"/>
-      <c r="EL1"/>
-      <c r="EM1"/>
-      <c r="EN1"/>
-      <c r="EO1"/>
-      <c r="EP1"/>
-      <c r="EQ1"/>
-      <c r="ER1"/>
-      <c r="ES1"/>
-      <c r="ET1"/>
-      <c r="EU1"/>
-      <c r="EV1"/>
-      <c r="EW1"/>
-      <c r="EX1"/>
-      <c r="EY1"/>
-      <c r="EZ1"/>
-      <c r="FA1"/>
-      <c r="FB1"/>
-      <c r="FC1"/>
-      <c r="FD1"/>
-      <c r="FE1"/>
-      <c r="FF1"/>
-      <c r="FG1"/>
-      <c r="FH1"/>
-      <c r="FI1"/>
-      <c r="FJ1"/>
-      <c r="FK1"/>
-      <c r="FL1"/>
-      <c r="FM1"/>
-      <c r="FN1"/>
-      <c r="FO1"/>
-      <c r="FP1"/>
-      <c r="FQ1"/>
-      <c r="FR1"/>
-      <c r="FS1"/>
-      <c r="FT1"/>
-      <c r="FU1"/>
-      <c r="FV1"/>
-      <c r="FW1"/>
-      <c r="FX1"/>
-      <c r="FY1"/>
-      <c r="FZ1"/>
-      <c r="GA1"/>
-      <c r="GB1"/>
-      <c r="GC1"/>
-      <c r="GD1"/>
-      <c r="GE1"/>
-      <c r="GF1"/>
-      <c r="GG1"/>
-      <c r="GH1"/>
-      <c r="GI1"/>
-      <c r="GJ1"/>
-      <c r="GK1"/>
-      <c r="GL1"/>
-      <c r="GM1"/>
-      <c r="GN1"/>
-      <c r="GO1"/>
-      <c r="GP1"/>
-      <c r="GQ1"/>
-      <c r="GR1"/>
-      <c r="GS1"/>
-      <c r="GT1"/>
-      <c r="GU1"/>
-      <c r="GV1"/>
-      <c r="GW1"/>
-      <c r="GX1"/>
-      <c r="GY1"/>
-      <c r="GZ1"/>
-      <c r="HA1"/>
-      <c r="HB1"/>
-      <c r="HC1"/>
-      <c r="HD1"/>
-      <c r="HE1"/>
-      <c r="HF1"/>
-      <c r="HG1"/>
-      <c r="HH1"/>
-      <c r="HI1"/>
-      <c r="HJ1"/>
-      <c r="HK1"/>
-      <c r="HL1"/>
-      <c r="HM1"/>
-      <c r="HN1"/>
-      <c r="HO1"/>
-      <c r="HP1"/>
-      <c r="HQ1"/>
-      <c r="HR1"/>
-      <c r="HS1"/>
-      <c r="HT1"/>
-      <c r="HU1"/>
-      <c r="HV1"/>
-      <c r="HW1"/>
-      <c r="HX1"/>
-      <c r="HY1"/>
-      <c r="HZ1"/>
-      <c r="IA1"/>
-      <c r="IB1"/>
-      <c r="IC1"/>
-      <c r="ID1"/>
-      <c r="IE1"/>
-      <c r="IF1"/>
-      <c r="IG1"/>
-      <c r="IH1"/>
-      <c r="II1"/>
-      <c r="IJ1"/>
-      <c r="IK1"/>
-      <c r="IL1"/>
-      <c r="IM1"/>
-      <c r="IN1"/>
-      <c r="IO1"/>
-      <c r="IP1"/>
-      <c r="IQ1"/>
-      <c r="IR1"/>
-      <c r="IS1"/>
-      <c r="IT1"/>
-      <c r="IU1"/>
-      <c r="IV1"/>
-      <c r="IW1"/>
-      <c r="IX1"/>
-      <c r="IY1"/>
-      <c r="IZ1"/>
-      <c r="JA1"/>
-      <c r="JB1"/>
-      <c r="JC1"/>
-      <c r="JD1"/>
-      <c r="JE1"/>
-      <c r="JF1"/>
-      <c r="JG1"/>
-      <c r="JH1"/>
-      <c r="JI1"/>
-      <c r="JJ1"/>
-      <c r="JK1"/>
-      <c r="JL1"/>
-      <c r="JM1"/>
-      <c r="JN1"/>
-      <c r="JO1"/>
-      <c r="JP1"/>
-      <c r="JQ1"/>
-      <c r="JR1"/>
-      <c r="JS1"/>
-      <c r="JT1"/>
-      <c r="JU1"/>
-      <c r="JV1"/>
-      <c r="JW1"/>
-      <c r="JX1"/>
-      <c r="JY1"/>
-      <c r="JZ1"/>
-      <c r="KA1"/>
-      <c r="KB1"/>
-      <c r="KC1"/>
-      <c r="KD1"/>
-      <c r="KE1"/>
-      <c r="KF1"/>
-      <c r="KG1"/>
-      <c r="KH1"/>
-      <c r="KI1"/>
-      <c r="KJ1"/>
-      <c r="KK1"/>
-      <c r="KL1"/>
-      <c r="KM1"/>
-      <c r="KN1"/>
-      <c r="KO1"/>
-      <c r="KP1"/>
-      <c r="KQ1"/>
-      <c r="KR1"/>
-      <c r="KS1"/>
-      <c r="KT1"/>
-      <c r="KU1"/>
-      <c r="KV1"/>
-      <c r="KW1"/>
-      <c r="KX1"/>
-      <c r="KY1"/>
-      <c r="KZ1"/>
-      <c r="LA1"/>
-      <c r="LB1"/>
-      <c r="LC1"/>
-      <c r="LD1"/>
-      <c r="LE1"/>
-      <c r="LF1"/>
-      <c r="LG1"/>
-      <c r="LH1"/>
-      <c r="LI1"/>
-      <c r="LJ1"/>
-      <c r="LK1"/>
-      <c r="LL1"/>
-      <c r="LM1"/>
-      <c r="LN1"/>
-      <c r="LO1"/>
-      <c r="LP1"/>
-      <c r="LQ1"/>
-      <c r="LR1"/>
-      <c r="LS1"/>
-      <c r="LT1"/>
-      <c r="LU1"/>
-      <c r="LV1"/>
-      <c r="LW1"/>
-      <c r="LX1"/>
-      <c r="LY1"/>
-      <c r="LZ1"/>
-      <c r="MA1"/>
-      <c r="MB1"/>
-      <c r="MC1"/>
-      <c r="MD1"/>
-      <c r="ME1"/>
-      <c r="MF1"/>
-      <c r="MG1"/>
-      <c r="MH1"/>
-      <c r="MI1"/>
-      <c r="MJ1"/>
-      <c r="MK1"/>
-      <c r="ML1"/>
-      <c r="MM1"/>
-      <c r="MN1"/>
-      <c r="MO1"/>
-      <c r="MP1"/>
-      <c r="MQ1"/>
-      <c r="MR1"/>
-      <c r="MS1"/>
-      <c r="MT1"/>
-      <c r="MU1"/>
-      <c r="MV1"/>
-      <c r="MW1"/>
-      <c r="MX1"/>
-      <c r="MY1"/>
-      <c r="MZ1"/>
-      <c r="NA1"/>
-      <c r="NB1"/>
-      <c r="NC1"/>
-      <c r="ND1"/>
-      <c r="NE1"/>
-      <c r="NF1"/>
-      <c r="NG1"/>
-      <c r="NH1"/>
-      <c r="NI1"/>
-      <c r="NJ1"/>
-      <c r="NK1"/>
-      <c r="NL1"/>
-      <c r="NM1"/>
-      <c r="NN1"/>
-      <c r="NO1"/>
-      <c r="NP1"/>
-      <c r="NQ1"/>
-      <c r="NR1"/>
-      <c r="NS1"/>
-      <c r="NT1"/>
-      <c r="NU1"/>
-      <c r="NV1"/>
-      <c r="NW1"/>
-      <c r="NX1"/>
-      <c r="NY1"/>
-      <c r="NZ1"/>
-      <c r="OA1"/>
-      <c r="OB1"/>
-      <c r="OC1"/>
-      <c r="OD1"/>
-      <c r="OE1"/>
-      <c r="OF1"/>
-      <c r="OG1"/>
-      <c r="OH1"/>
-      <c r="OI1"/>
-      <c r="OJ1"/>
-      <c r="OK1"/>
-      <c r="OL1"/>
-      <c r="OM1"/>
-      <c r="ON1"/>
-      <c r="OO1"/>
-      <c r="OP1"/>
-      <c r="OQ1"/>
-      <c r="OR1"/>
-      <c r="OS1"/>
-      <c r="OT1"/>
-      <c r="OU1"/>
-      <c r="OV1"/>
-      <c r="OW1"/>
-      <c r="OX1"/>
-      <c r="OY1"/>
-      <c r="OZ1"/>
-      <c r="PA1"/>
-      <c r="PB1"/>
-      <c r="PC1"/>
-      <c r="PD1"/>
-      <c r="PE1"/>
-      <c r="PF1"/>
-      <c r="PG1"/>
-      <c r="PH1"/>
-      <c r="PI1"/>
-      <c r="PJ1"/>
-      <c r="PK1"/>
-      <c r="PL1"/>
-      <c r="PM1"/>
-      <c r="PN1"/>
-      <c r="PO1"/>
-      <c r="PP1"/>
-      <c r="PQ1"/>
-      <c r="PR1"/>
-      <c r="PS1"/>
-      <c r="PT1"/>
-      <c r="PU1"/>
-      <c r="PV1"/>
-      <c r="PW1"/>
-      <c r="PX1"/>
-      <c r="PY1"/>
-      <c r="PZ1"/>
-      <c r="QA1"/>
-      <c r="QB1"/>
-      <c r="QC1"/>
-      <c r="QD1"/>
-      <c r="QE1"/>
-      <c r="QF1"/>
-      <c r="QG1"/>
-      <c r="QH1"/>
-      <c r="QI1"/>
-      <c r="QJ1"/>
-      <c r="QK1"/>
-      <c r="QL1"/>
-      <c r="QM1"/>
-      <c r="QN1"/>
-      <c r="QO1"/>
-      <c r="QP1"/>
-      <c r="QQ1"/>
-      <c r="QR1"/>
-      <c r="QS1"/>
-      <c r="QT1"/>
-      <c r="QU1"/>
-      <c r="QV1"/>
-      <c r="QW1"/>
-      <c r="QX1"/>
-      <c r="QY1"/>
-      <c r="QZ1"/>
-      <c r="RA1"/>
-      <c r="RB1"/>
-      <c r="RC1"/>
-      <c r="RD1"/>
-      <c r="RE1"/>
-      <c r="RF1"/>
-      <c r="RG1"/>
-      <c r="RH1"/>
-      <c r="RI1"/>
-      <c r="RJ1"/>
-      <c r="RK1"/>
-      <c r="RL1"/>
-      <c r="RM1"/>
-      <c r="RN1"/>
-      <c r="RO1"/>
-      <c r="RP1"/>
-      <c r="RQ1"/>
-      <c r="RR1"/>
-      <c r="RS1"/>
-      <c r="RT1"/>
-      <c r="RU1"/>
-      <c r="RV1"/>
-      <c r="RW1"/>
-      <c r="RX1"/>
-      <c r="RY1"/>
-      <c r="RZ1"/>
-      <c r="SA1"/>
-      <c r="SB1"/>
-      <c r="SC1"/>
-      <c r="SD1"/>
-      <c r="SE1"/>
-      <c r="SF1"/>
-      <c r="SG1"/>
-      <c r="SH1"/>
-      <c r="SI1"/>
-      <c r="SJ1"/>
-      <c r="SK1"/>
-      <c r="SL1"/>
-      <c r="SM1"/>
-      <c r="SN1"/>
-      <c r="SO1"/>
-      <c r="SP1"/>
-      <c r="SQ1"/>
-      <c r="SR1"/>
-      <c r="SS1"/>
-      <c r="ST1"/>
-      <c r="SU1"/>
-      <c r="SV1"/>
-      <c r="SW1"/>
-      <c r="SX1"/>
-      <c r="SY1"/>
-      <c r="SZ1"/>
-      <c r="TA1"/>
-      <c r="TB1"/>
-      <c r="TC1"/>
-      <c r="TD1"/>
-      <c r="TE1"/>
-      <c r="TF1"/>
-      <c r="TG1"/>
-      <c r="TH1"/>
-      <c r="TI1"/>
-      <c r="TJ1"/>
-      <c r="TK1"/>
-      <c r="TL1"/>
-      <c r="TM1"/>
-      <c r="TN1"/>
-      <c r="TO1"/>
-      <c r="TP1"/>
-      <c r="TQ1"/>
-      <c r="TR1"/>
-      <c r="TS1"/>
-      <c r="TT1"/>
-      <c r="TU1"/>
-      <c r="TV1"/>
-      <c r="TW1"/>
-      <c r="TX1"/>
-      <c r="TY1"/>
-      <c r="TZ1"/>
-      <c r="UA1"/>
-      <c r="UB1"/>
-      <c r="UC1"/>
-      <c r="UD1"/>
-      <c r="UE1"/>
-      <c r="UF1"/>
-      <c r="UG1"/>
-      <c r="UH1"/>
-      <c r="UI1"/>
-      <c r="UJ1"/>
-      <c r="UK1"/>
-      <c r="UL1"/>
-      <c r="UM1"/>
-      <c r="UN1"/>
-      <c r="UO1"/>
-      <c r="UP1"/>
-      <c r="UQ1"/>
-      <c r="UR1"/>
-      <c r="US1"/>
-      <c r="UT1"/>
-      <c r="UU1"/>
-      <c r="UV1"/>
-      <c r="UW1"/>
-      <c r="UX1"/>
-      <c r="UY1"/>
-      <c r="UZ1"/>
-      <c r="VA1"/>
-      <c r="VB1"/>
-      <c r="VC1"/>
-      <c r="VD1"/>
-      <c r="VE1"/>
-      <c r="VF1"/>
-      <c r="VG1"/>
-      <c r="VH1"/>
-      <c r="VI1"/>
-      <c r="VJ1"/>
-      <c r="VK1"/>
-      <c r="VL1"/>
-      <c r="VM1"/>
-      <c r="VN1"/>
-      <c r="VO1"/>
-      <c r="VP1"/>
-      <c r="VQ1"/>
-      <c r="VR1"/>
-      <c r="VS1"/>
-      <c r="VT1"/>
-      <c r="VU1"/>
-      <c r="VV1"/>
-      <c r="VW1"/>
-      <c r="VX1"/>
-      <c r="VY1"/>
-      <c r="VZ1"/>
-      <c r="WA1"/>
-      <c r="WB1"/>
-      <c r="WC1"/>
-      <c r="WD1"/>
-      <c r="WE1"/>
-      <c r="WF1"/>
-      <c r="WG1"/>
-      <c r="WH1"/>
-      <c r="WI1"/>
-      <c r="WJ1"/>
-      <c r="WK1"/>
-      <c r="WL1"/>
-      <c r="WM1"/>
-      <c r="WN1"/>
-      <c r="WO1"/>
-      <c r="WP1"/>
-      <c r="WQ1"/>
-      <c r="WR1"/>
-      <c r="WS1"/>
-      <c r="WT1"/>
-      <c r="WU1"/>
-      <c r="WV1"/>
-      <c r="WW1"/>
-      <c r="WX1"/>
-      <c r="WY1"/>
-      <c r="WZ1"/>
-      <c r="XA1"/>
-      <c r="XB1"/>
-      <c r="XC1"/>
-      <c r="XD1"/>
-      <c r="XE1"/>
-      <c r="XF1"/>
-      <c r="XG1"/>
-      <c r="XH1"/>
-      <c r="XI1"/>
-      <c r="XJ1"/>
-      <c r="XK1"/>
-      <c r="XL1"/>
-      <c r="XM1"/>
-      <c r="XN1"/>
-      <c r="XO1"/>
-      <c r="XP1"/>
-      <c r="XQ1"/>
-      <c r="XR1"/>
-      <c r="XS1"/>
-      <c r="XT1"/>
-      <c r="XU1"/>
-      <c r="XV1"/>
-      <c r="XW1"/>
-      <c r="XX1"/>
-      <c r="XY1"/>
-      <c r="XZ1"/>
-      <c r="YA1"/>
-      <c r="YB1"/>
-      <c r="YC1"/>
-      <c r="YD1"/>
-      <c r="YE1"/>
-      <c r="YF1"/>
-      <c r="YG1"/>
-      <c r="YH1"/>
-      <c r="YI1"/>
-      <c r="YJ1"/>
-      <c r="YK1"/>
-      <c r="YL1"/>
-      <c r="YM1"/>
-      <c r="YN1"/>
-      <c r="YO1"/>
-      <c r="YP1"/>
-      <c r="YQ1"/>
-      <c r="YR1"/>
-      <c r="YS1"/>
-      <c r="YT1"/>
-      <c r="YU1"/>
-      <c r="YV1"/>
-      <c r="YW1"/>
-      <c r="YX1"/>
-      <c r="YY1"/>
-      <c r="YZ1"/>
-      <c r="ZA1"/>
-      <c r="ZB1"/>
-      <c r="ZC1"/>
-      <c r="ZD1"/>
-      <c r="ZE1"/>
-      <c r="ZF1"/>
-      <c r="ZG1"/>
-      <c r="ZH1"/>
-      <c r="ZI1"/>
-      <c r="ZJ1"/>
-      <c r="ZK1"/>
-      <c r="ZL1"/>
-      <c r="ZM1"/>
-      <c r="ZN1"/>
-      <c r="ZO1"/>
-      <c r="ZP1"/>
-      <c r="ZQ1"/>
-      <c r="ZR1"/>
-      <c r="ZS1"/>
-      <c r="ZT1"/>
-      <c r="ZU1"/>
-      <c r="ZV1"/>
-      <c r="ZW1"/>
-      <c r="ZX1"/>
-      <c r="ZY1"/>
-      <c r="ZZ1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>